<commit_message>
Move run_checker_framework.bat to new folder
</commit_message>
<xml_diff>
--- a/data/checker_framework_data.xlsx
+++ b/data/checker_framework_data.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="51">
   <si>
     <t>[argument] incompatible argument for parameter arg1 of arraycopy.</t>
   </si>
@@ -67,6 +67,9 @@
     <t>[array.length.negative] Variable used in array creation could be negative.</t>
   </si>
   <si>
+    <t>[dep-ann] deprecated item is not annotated with @Deprecated</t>
+  </si>
+  <si>
     <t>[format.string] invalid format string (is a @Format annotation missing?)</t>
   </si>
   <si>
@@ -79,13 +82,13 @@
     <t>[required.method.not.called] @MustCall method close may not have been invoked on stream or any of its aliases.</t>
   </si>
   <si>
-    <t>[required.method.not.called] @MustCall method close may not have been invoked on temp-var-106 or any of its aliases.</t>
-  </si>
-  <si>
-    <t>[required.method.not.called] @MustCall method close may not have been invoked on temp-var-109 or any of its aliases.</t>
-  </si>
-  <si>
-    <t>[required.method.not.called] @MustCall method close may not have been invoked on temp-var-286 or any of its aliases.</t>
+    <t>[required.method.not.called] @MustCall method close may not have been invoked on temp-var-145 or any of its aliases.</t>
+  </si>
+  <si>
+    <t>[required.method.not.called] @MustCall method close may not have been invoked on temp-var-148 or any of its aliases.</t>
+  </si>
+  <si>
+    <t>[required.method.not.called] @MustCall method close may not have been invoked on temp-var-325 or any of its aliases.</t>
   </si>
   <si>
     <t>[return] incompatible types in return.</t>
@@ -137,6 +140,9 @@
   </si>
   <si>
     <t>COG Dataset 3 - 63</t>
+  </si>
+  <si>
+    <t>COG Dataset 3 - 7</t>
   </si>
   <si>
     <t>COG Dataset 3 - 70</t>
@@ -518,15 +524,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:Z24"/>
+  <dimension ref="A1:AA25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:26">
+    <row r="1" spans="1:27">
       <c r="A1" s="1" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>0</v>
@@ -603,26 +609,29 @@
       <c r="Z1" s="1" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="2" spans="1:26">
+      <c r="AA1" s="1" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="2" spans="1:27">
       <c r="A2" s="1" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="G2">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:26">
+    <row r="3" spans="1:27">
       <c r="A3" s="1" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="P3">
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:26">
+    <row r="4" spans="1:27">
       <c r="A4" s="1" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="E4">
         <v>1</v>
@@ -631,39 +640,39 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:26">
+    <row r="5" spans="1:27">
       <c r="A5" s="1" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="L5">
         <v>1</v>
       </c>
-      <c r="Z5">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="6" spans="1:26">
+      <c r="AA5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:27">
       <c r="A6" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="W6">
-        <v>1</v>
+        <v>31</v>
       </c>
       <c r="X6">
         <v>1</v>
       </c>
-    </row>
-    <row r="7" spans="1:26">
+      <c r="Y6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:27">
       <c r="A7" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="U7">
+        <v>32</v>
+      </c>
+      <c r="V7">
         <v>4</v>
       </c>
     </row>
-    <row r="8" spans="1:26">
+    <row r="8" spans="1:27">
       <c r="A8" s="1" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="B8">
         <v>2</v>
@@ -675,9 +684,9 @@
         <v>6</v>
       </c>
     </row>
-    <row r="9" spans="1:26">
+    <row r="9" spans="1:27">
       <c r="A9" s="1" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="E9">
         <v>2</v>
@@ -689,28 +698,28 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:26">
+    <row r="10" spans="1:27">
       <c r="A10" s="1" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="H10">
         <v>1</v>
       </c>
-      <c r="T10">
+      <c r="U10">
         <v>2</v>
       </c>
     </row>
-    <row r="11" spans="1:26">
+    <row r="11" spans="1:27">
       <c r="A11" s="1" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="R11">
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:26">
+    <row r="12" spans="1:27">
       <c r="A12" s="1" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="L12">
         <v>1</v>
@@ -722,111 +731,119 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:26">
+    <row r="13" spans="1:27">
       <c r="A13" s="1" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="K13">
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:26">
+    <row r="14" spans="1:27">
       <c r="A14" s="1" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="J14">
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:26">
+    <row r="15" spans="1:27">
       <c r="A15" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="S15">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="16" spans="1:26">
+        <v>40</v>
+      </c>
+      <c r="T15">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:27">
       <c r="A16" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="Z16">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="17" spans="1:26">
+        <v>41</v>
+      </c>
+      <c r="AA16">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="1:27">
       <c r="A17" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="I17">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="18" spans="1:26">
+        <v>42</v>
+      </c>
+      <c r="S17">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="1:27">
       <c r="A18" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="V18">
-        <v>1</v>
-      </c>
-      <c r="Y18">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="19" spans="1:26">
+        <v>43</v>
+      </c>
+      <c r="I18">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="1:27">
       <c r="A19" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="O19">
+        <v>44</v>
+      </c>
+      <c r="W19">
+        <v>1</v>
+      </c>
+      <c r="Z19">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" spans="1:27">
+      <c r="A20" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="O20">
         <v>3</v>
       </c>
-      <c r="P19">
+      <c r="P20">
         <v>3</v>
       </c>
-      <c r="Q19">
+      <c r="Q20">
         <v>3</v>
       </c>
     </row>
-    <row r="20" spans="1:26">
-      <c r="A20" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="U20">
+    <row r="21" spans="1:27">
+      <c r="A21" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="V21">
         <v>2</v>
       </c>
     </row>
-    <row r="21" spans="1:26">
-      <c r="A21" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="P21">
+    <row r="22" spans="1:27">
+      <c r="A22" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="P22">
         <v>2</v>
       </c>
-      <c r="Q21">
+      <c r="Q22">
         <v>2</v>
       </c>
     </row>
-    <row r="22" spans="1:26">
-      <c r="A22" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="G22">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="23" spans="1:26">
+    <row r="23" spans="1:27">
       <c r="A23" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="Z23">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="24" spans="1:26">
+        <v>48</v>
+      </c>
+      <c r="G23">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="24" spans="1:27">
       <c r="A24" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="G24">
+        <v>49</v>
+      </c>
+      <c r="AA24">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="25" spans="1:27">
+      <c r="A25" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="G25">
         <v>1</v>
       </c>
     </row>

</xml_diff>